<commit_message>
Analyze data for ashwani tomorrow.
</commit_message>
<xml_diff>
--- a/stimuli/3Dec2015.xlsx
+++ b/stimuli/3Dec2015.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10848" windowHeight="6396" tabRatio="981"/>
+    <workbookView xWindow="12480" yWindow="-120" windowWidth="10848" windowHeight="6396" tabRatio="981"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -398,7 +398,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D4"/>
+      <selection activeCell="D2" sqref="D2:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,11 +448,11 @@
         <v>5</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D13" si="0">A2+C2</f>
+        <f>A2+C2</f>
         <v>10</v>
       </c>
       <c r="E2" s="3">
-        <f t="shared" ref="E2:E13" si="1">B2+C2</f>
+        <f>B2+C2</f>
         <v>11</v>
       </c>
       <c r="F2" s="4">
@@ -467,55 +467,55 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>A3+C3</f>
+        <v>24</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f>B3+C3</f>
+        <v>26</v>
       </c>
       <c r="F3" s="4">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="G3" s="3">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="H3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" si="0"/>
+        <f>A4+C4</f>
         <v>24</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" si="1"/>
-        <v>26</v>
+        <f>B4+C4</f>
+        <v>28</v>
       </c>
       <c r="F4" s="3">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="G4" s="3">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="H4" s="3">
         <v>1</v>
@@ -523,55 +523,55 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3">
+        <f>A5+C5</f>
+        <v>6</v>
+      </c>
+      <c r="E5" s="3">
+        <f>B5+C5</f>
         <v>7</v>
       </c>
-      <c r="B5" s="3">
-        <v>21</v>
-      </c>
-      <c r="C5" s="3">
-        <v>17</v>
-      </c>
-      <c r="D5" s="3">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="E5" s="3">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
       <c r="F5" s="3">
-        <v>122</v>
+        <v>170</v>
       </c>
       <c r="G5" s="3">
-        <v>127</v>
+        <v>171</v>
       </c>
       <c r="H5" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <f>A6+C6</f>
+        <v>42</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="1"/>
-        <v>28</v>
+        <f>B6+C6</f>
+        <v>47</v>
       </c>
       <c r="F6" s="3">
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="G6" s="3">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
@@ -579,83 +579,83 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <f>A7+C7</f>
+        <v>40</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" si="1"/>
-        <v>36</v>
+        <f>B7+C7</f>
+        <v>45</v>
       </c>
       <c r="F7" s="3">
+        <v>140</v>
+      </c>
+      <c r="G7" s="3">
         <v>144</v>
       </c>
-      <c r="G7" s="3">
-        <v>149</v>
-      </c>
       <c r="H7" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3">
         <v>5</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>A8+C8</f>
+        <v>10</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f>B8+C8</f>
+        <v>20</v>
       </c>
       <c r="F8" s="3">
-        <v>170</v>
+        <v>105</v>
       </c>
       <c r="G8" s="3">
-        <v>171</v>
+        <v>106</v>
       </c>
       <c r="H8" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>A9+C9</f>
+        <v>24</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <f>B9+C9</f>
+        <v>38</v>
       </c>
       <c r="F9" s="3">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="G9" s="3">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="H9" s="3">
         <v>2</v>
@@ -663,55 +663,55 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" si="0"/>
-        <v>42</v>
+        <f>A10+C10</f>
+        <v>24</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" si="1"/>
-        <v>47</v>
+        <f>B10+C10</f>
+        <v>36</v>
       </c>
       <c r="F10" s="3">
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="G10" s="3">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="H10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B11" s="3">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="0"/>
-        <v>42</v>
+        <f>A11+C11</f>
+        <v>6</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="1"/>
-        <v>62</v>
+        <f>B11+C11</f>
+        <v>15</v>
       </c>
       <c r="F11" s="3">
-        <v>108</v>
+        <v>170</v>
       </c>
       <c r="G11" s="3">
-        <v>114</v>
+        <v>171</v>
       </c>
       <c r="H11" s="3">
         <v>2</v>
@@ -719,30 +719,30 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C12" s="3">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>A12+C12</f>
+        <v>42</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="1"/>
-        <v>45</v>
+        <f>B12+C12</f>
+        <v>62</v>
       </c>
       <c r="F12" s="3">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="G12" s="3">
-        <v>144</v>
+        <v>114</v>
       </c>
       <c r="H12" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -756,11 +756,11 @@
         <v>25</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="0"/>
+        <f>A13+C13</f>
         <v>40</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="1"/>
+        <f>B13+C13</f>
         <v>100</v>
       </c>
       <c r="F13" s="3">
@@ -774,6 +774,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:H13">
+    <sortCondition ref="H1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>